<commit_message>
change query and run anaylise_rest file for change the excel file
</commit_message>
<xml_diff>
--- a/excel_data/orders_and_products.xlsx
+++ b/excel_data/orders_and_products.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="88">
   <si>
     <t>Order_item_id</t>
   </si>
@@ -26,12 +26,6 @@
   </si>
   <si>
     <t>price</t>
-  </si>
-  <si>
-    <t>order_date</t>
-  </si>
-  <si>
-    <t>order_time</t>
   </si>
   <si>
     <t>number_of_orders_by_item</t>
@@ -290,9 +284,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
-  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -345,13 +336,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -646,13 +635,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -671,843 +660,645 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" s="2">
-        <v>44927</v>
-      </c>
-      <c r="F2" s="3">
-        <v>0.5653587962962963</v>
-      </c>
-      <c r="G2">
+        <v>42</v>
+      </c>
+      <c r="E2">
         <v>470</v>
       </c>
-      <c r="H2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="F2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>108</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="2">
-        <v>44927</v>
-      </c>
-      <c r="F3" s="3">
-        <v>0.4983796296296296</v>
-      </c>
-      <c r="G3">
+        <v>43</v>
+      </c>
+      <c r="E3">
         <v>562</v>
       </c>
-      <c r="H3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="F3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="2">
-        <v>44927</v>
-      </c>
-      <c r="F4" s="3">
-        <v>0.5437384259259259</v>
-      </c>
-      <c r="G4">
+        <v>44</v>
+      </c>
+      <c r="E4">
         <v>583</v>
       </c>
-      <c r="H4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="F4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>101</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" s="2">
-        <v>44927</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0.5205555555555555</v>
-      </c>
-      <c r="G5">
+        <v>45</v>
+      </c>
+      <c r="E5">
         <v>622</v>
       </c>
-      <c r="H5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="F5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>107</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="2">
-        <v>44927</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0.5645833333333333</v>
-      </c>
-      <c r="G6">
+        <v>46</v>
+      </c>
+      <c r="E6">
         <v>456</v>
       </c>
-      <c r="H6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="F6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>132</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" s="2">
-        <v>44927</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0.5361226851851851</v>
-      </c>
-      <c r="G7">
+        <v>47</v>
+      </c>
+      <c r="E7">
         <v>420</v>
       </c>
-      <c r="H7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="F7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>120</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="2">
-        <v>44927</v>
-      </c>
-      <c r="F8" s="3">
-        <v>0.5827430555555555</v>
-      </c>
-      <c r="G8">
+        <v>44</v>
+      </c>
+      <c r="E8">
         <v>489</v>
       </c>
-      <c r="H8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="F8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>131</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="2">
-        <v>44927</v>
-      </c>
-      <c r="F9" s="3">
-        <v>0.5784722222222223</v>
-      </c>
-      <c r="G9">
+        <v>42</v>
+      </c>
+      <c r="E9">
         <v>364</v>
       </c>
-      <c r="H9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="F9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>110</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="2">
-        <v>44927</v>
-      </c>
-      <c r="F10" s="3">
-        <v>0.5361226851851851</v>
-      </c>
-      <c r="G10">
+        <v>42</v>
+      </c>
+      <c r="E10">
         <v>360</v>
       </c>
-      <c r="H10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="F10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>117</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="2">
-        <v>44927</v>
-      </c>
-      <c r="F11" s="3">
-        <v>0.4983796296296296</v>
-      </c>
-      <c r="G11">
+        <v>45</v>
+      </c>
+      <c r="E11">
         <v>455</v>
       </c>
-      <c r="H11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="F11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>129</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="2">
-        <v>44927</v>
-      </c>
-      <c r="F12" s="3">
-        <v>0.4983796296296296</v>
-      </c>
-      <c r="G12">
+        <v>48</v>
+      </c>
+      <c r="E12">
         <v>359</v>
       </c>
-      <c r="H12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="F12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>124</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="2">
-        <v>44927</v>
-      </c>
-      <c r="F13" s="3">
-        <v>0.4983796296296296</v>
-      </c>
-      <c r="G13">
+        <v>43</v>
+      </c>
+      <c r="E13">
         <v>367</v>
       </c>
-      <c r="H13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="F13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>118</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
-      </c>
-      <c r="E14" s="2">
-        <v>44927</v>
-      </c>
-      <c r="F14" s="3">
-        <v>0.5784722222222223</v>
-      </c>
-      <c r="G14">
+        <v>49</v>
+      </c>
+      <c r="E14">
         <v>354</v>
       </c>
-      <c r="H14" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="F14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>127</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D15" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="2">
-        <v>44927</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0.5784722222222223</v>
-      </c>
-      <c r="G15">
+        <v>42</v>
+      </c>
+      <c r="E15">
         <v>273</v>
       </c>
-      <c r="H15" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="F15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>112</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="2">
-        <v>44927</v>
-      </c>
-      <c r="F16" s="3">
-        <v>0.6889351851851852</v>
-      </c>
-      <c r="G16">
+        <v>49</v>
+      </c>
+      <c r="E16">
         <v>324</v>
       </c>
-      <c r="H16" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="F16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>130</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" s="2">
-        <v>44927</v>
-      </c>
-      <c r="F17" s="3">
-        <v>0.5361226851851851</v>
-      </c>
-      <c r="G17">
+        <v>50</v>
+      </c>
+      <c r="E17">
         <v>239</v>
       </c>
-      <c r="H17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="F17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>119</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D18" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" s="2">
-        <v>44927</v>
-      </c>
-      <c r="F18" s="3">
-        <v>0.5086574074074074</v>
-      </c>
-      <c r="G18">
+        <v>51</v>
+      </c>
+      <c r="E18">
         <v>379</v>
       </c>
-      <c r="H18" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="F18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>111</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D19" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" s="2">
-        <v>44927</v>
-      </c>
-      <c r="F19" s="3">
-        <v>0.5653587962962963</v>
-      </c>
-      <c r="G19">
+        <v>51</v>
+      </c>
+      <c r="E19">
         <v>355</v>
       </c>
-      <c r="H19" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="F19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>106</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D20" t="s">
-        <v>54</v>
-      </c>
-      <c r="E20" s="2">
-        <v>44927</v>
-      </c>
-      <c r="F20" s="3">
-        <v>0.4983796296296296</v>
-      </c>
-      <c r="G20">
+        <v>52</v>
+      </c>
+      <c r="E20">
         <v>571</v>
       </c>
-      <c r="H20" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="F20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21">
         <v>126</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D21" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" s="2">
-        <v>44927</v>
-      </c>
-      <c r="F21" s="3">
-        <v>0.5361226851851851</v>
-      </c>
-      <c r="G21">
+        <v>43</v>
+      </c>
+      <c r="E21">
         <v>249</v>
       </c>
-      <c r="H21" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="F21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22">
         <v>105</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D22" t="s">
-        <v>54</v>
-      </c>
-      <c r="E22" s="2">
-        <v>44927</v>
-      </c>
-      <c r="F22" s="3">
-        <v>0.5418402777777778</v>
-      </c>
-      <c r="G22">
+        <v>52</v>
+      </c>
+      <c r="E22">
         <v>463</v>
       </c>
-      <c r="H22" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="F22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23">
         <v>122</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C23" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D23" t="s">
-        <v>54</v>
-      </c>
-      <c r="E23" s="2">
-        <v>44927</v>
-      </c>
-      <c r="F23" s="3">
-        <v>0.5361226851851851</v>
-      </c>
-      <c r="G23">
+        <v>52</v>
+      </c>
+      <c r="E23">
         <v>461</v>
       </c>
-      <c r="H23" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="F23" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24">
         <v>128</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D24" t="s">
-        <v>50</v>
-      </c>
-      <c r="E24" s="2">
-        <v>44927</v>
-      </c>
-      <c r="F24" s="3">
-        <v>0.5784722222222223</v>
-      </c>
-      <c r="G24">
+        <v>48</v>
+      </c>
+      <c r="E24">
         <v>207</v>
       </c>
-      <c r="H24" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="F24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25">
         <v>113</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D25" t="s">
-        <v>55</v>
-      </c>
-      <c r="E25" s="2">
-        <v>44927</v>
-      </c>
-      <c r="F25" s="3">
-        <v>0.5437384259259259</v>
-      </c>
-      <c r="G25">
+        <v>53</v>
+      </c>
+      <c r="E25">
         <v>620</v>
       </c>
-      <c r="H25" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="F25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26">
         <v>116</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D26" t="s">
-        <v>46</v>
-      </c>
-      <c r="E26" s="2">
-        <v>44927</v>
-      </c>
-      <c r="F26" s="3">
-        <v>0.5784722222222223</v>
-      </c>
-      <c r="G26">
+        <v>44</v>
+      </c>
+      <c r="E26">
         <v>214</v>
       </c>
-      <c r="H26" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="F26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27">
         <v>104</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C27" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D27" t="s">
-        <v>56</v>
-      </c>
-      <c r="E27" s="2">
-        <v>44927</v>
-      </c>
-      <c r="F27" s="3">
-        <v>0.5449189814814814</v>
-      </c>
-      <c r="G27">
+        <v>54</v>
+      </c>
+      <c r="E27">
         <v>238</v>
       </c>
-      <c r="H27" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="F27" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28">
         <v>121</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C28" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D28" t="s">
-        <v>56</v>
-      </c>
-      <c r="E28" s="2">
-        <v>44927</v>
-      </c>
-      <c r="F28" s="3">
-        <v>0.5645833333333333</v>
-      </c>
-      <c r="G28">
+        <v>54</v>
+      </c>
+      <c r="E28">
         <v>233</v>
       </c>
-      <c r="H28" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="F28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29">
         <v>103</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D29" t="s">
-        <v>57</v>
-      </c>
-      <c r="E29" s="2">
-        <v>44927</v>
-      </c>
-      <c r="F29" s="3">
-        <v>0.6498379629629629</v>
-      </c>
-      <c r="G29">
+        <v>55</v>
+      </c>
+      <c r="E29">
         <v>257</v>
       </c>
-      <c r="H29" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="F29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30">
         <v>123</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C30" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E30" s="2">
-        <v>44927</v>
-      </c>
-      <c r="F30" s="3">
-        <v>0.535150462962963</v>
-      </c>
-      <c r="G30">
+        <v>55</v>
+      </c>
+      <c r="E30">
         <v>237</v>
       </c>
-      <c r="H30" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="F30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31">
         <v>109</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C31" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D31" t="s">
-        <v>44</v>
-      </c>
-      <c r="E31" s="2">
-        <v>44927</v>
-      </c>
-      <c r="F31" s="3">
-        <v>0.4851388888888889</v>
-      </c>
-      <c r="G31">
+        <v>42</v>
+      </c>
+      <c r="E31">
         <v>588</v>
       </c>
-      <c r="H31" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+      <c r="F31" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32">
         <v>114</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C32" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D32" t="s">
-        <v>57</v>
-      </c>
-      <c r="E32" s="2">
-        <v>44927</v>
-      </c>
-      <c r="F32" s="3">
-        <v>0.5205555555555555</v>
-      </c>
-      <c r="G32">
+        <v>55</v>
+      </c>
+      <c r="E32">
         <v>205</v>
       </c>
-      <c r="H32" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="F32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33">
         <v>115</v>
       </c>
       <c r="B33" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C33" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D33" t="s">
-        <v>53</v>
-      </c>
-      <c r="E33" s="2">
-        <v>44929</v>
-      </c>
-      <c r="F33" s="3">
-        <v>0.7848379629629629</v>
-      </c>
-      <c r="G33">
+        <v>51</v>
+      </c>
+      <c r="E33">
         <v>123</v>
       </c>
-      <c r="H33" t="s">
-        <v>89</v>
+      <c r="F33" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create a new query for we can see the income by category with making the new sheet in same excel
</commit_message>
<xml_diff>
--- a/excel_data/orders_and_products.xlsx
+++ b/excel_data/orders_and_products.xlsx
@@ -7,14 +7,15 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="income" sheetId="1" r:id="rId1"/>
+    <sheet name="income_by_category" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="92">
   <si>
     <t>Order_item_id</t>
   </si>
@@ -278,6 +279,18 @@
   </si>
   <si>
     <t>$1,469.85</t>
+  </si>
+  <si>
+    <t>$62,286.50</t>
+  </si>
+  <si>
+    <t>$42,746.00</t>
+  </si>
+  <si>
+    <t>$38,137.75</t>
+  </si>
+  <si>
+    <t>$19,138.00</t>
   </si>
 </sst>
 </file>
@@ -1304,4 +1317,72 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2">
+        <v>3470</v>
+      </c>
+      <c r="C2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3">
+        <v>2948</v>
+      </c>
+      <c r="C3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4">
+        <v>2945</v>
+      </c>
+      <c r="C4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5">
+        <v>2734</v>
+      </c>
+      <c r="C5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
create a query for charges & passive for can see all money movments
</commit_message>
<xml_diff>
--- a/excel_data/orders_and_products.xlsx
+++ b/excel_data/orders_and_products.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="income" sheetId="1" r:id="rId1"/>
     <sheet name="income_by_category" sheetId="2" r:id="rId2"/>
+    <sheet name="charges&amp;passive" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="158">
   <si>
     <t>Order_item_id</t>
   </si>
@@ -35,6 +36,9 @@
     <t>income</t>
   </si>
   <si>
+    <t>Korean Beef Bowl</t>
+  </si>
+  <si>
     <t>Spaghetti &amp; Meatballs</t>
   </si>
   <si>
@@ -122,21 +126,18 @@
     <t>Chips &amp; Guacamole</t>
   </si>
   <si>
-    <t>Korean Beef Bowl</t>
-  </si>
-  <si>
     <t>Potstickers</t>
   </si>
   <si>
     <t>Chicken Tacos</t>
   </si>
   <si>
+    <t>Asian</t>
+  </si>
+  <si>
     <t>Italian</t>
   </si>
   <si>
-    <t>Asian</t>
-  </si>
-  <si>
     <t>American</t>
   </si>
   <si>
@@ -185,6 +186,9 @@
     <t>9.00</t>
   </si>
   <si>
+    <t>$10,554.60</t>
+  </si>
+  <si>
     <t>$8,436.50</t>
   </si>
   <si>
@@ -272,9 +276,6 @@
     <t>$2,133.00</t>
   </si>
   <si>
-    <t>$10,554.60</t>
-  </si>
-  <si>
     <t>$1,845.00</t>
   </si>
   <si>
@@ -291,6 +292,204 @@
   </si>
   <si>
     <t>$19,138.00</t>
+  </si>
+  <si>
+    <t>chargers</t>
+  </si>
+  <si>
+    <t>passive</t>
+  </si>
+  <si>
+    <t>$4,749.57</t>
+  </si>
+  <si>
+    <t>$3,796.43</t>
+  </si>
+  <si>
+    <t>$3,667.05</t>
+  </si>
+  <si>
+    <t>$3,659.78</t>
+  </si>
+  <si>
+    <t>$3,624.71</t>
+  </si>
+  <si>
+    <t>$3,385.80</t>
+  </si>
+  <si>
+    <t>$3,203.55</t>
+  </si>
+  <si>
+    <t>$3,069.70</t>
+  </si>
+  <si>
+    <t>$2,940.21</t>
+  </si>
+  <si>
+    <t>$2,907.90</t>
+  </si>
+  <si>
+    <t>$2,651.51</t>
+  </si>
+  <si>
+    <t>$2,504.03</t>
+  </si>
+  <si>
+    <t>$2,394.68</t>
+  </si>
+  <si>
+    <t>$2,381.54</t>
+  </si>
+  <si>
+    <t>$2,205.16</t>
+  </si>
+  <si>
+    <t>$2,179.71</t>
+  </si>
+  <si>
+    <t>$2,145.62</t>
+  </si>
+  <si>
+    <t>$2,038.07</t>
+  </si>
+  <si>
+    <t>$1,909.01</t>
+  </si>
+  <si>
+    <t>$1,798.65</t>
+  </si>
+  <si>
+    <t>$1,624.73</t>
+  </si>
+  <si>
+    <t>$1,458.45</t>
+  </si>
+  <si>
+    <t>$1,452.15</t>
+  </si>
+  <si>
+    <t>$1,443.83</t>
+  </si>
+  <si>
+    <t>$1,395.00</t>
+  </si>
+  <si>
+    <t>$1,343.39</t>
+  </si>
+  <si>
+    <t>$1,124.55</t>
+  </si>
+  <si>
+    <t>$1,100.93</t>
+  </si>
+  <si>
+    <t>$1,040.85</t>
+  </si>
+  <si>
+    <t>$959.85</t>
+  </si>
+  <si>
+    <t>$830.25</t>
+  </si>
+  <si>
+    <t>$661.43</t>
+  </si>
+  <si>
+    <t>$5,805.03</t>
+  </si>
+  <si>
+    <t>$4,640.08</t>
+  </si>
+  <si>
+    <t>$4,481.95</t>
+  </si>
+  <si>
+    <t>$4,473.07</t>
+  </si>
+  <si>
+    <t>$4,430.20</t>
+  </si>
+  <si>
+    <t>$4,138.20</t>
+  </si>
+  <si>
+    <t>$3,915.45</t>
+  </si>
+  <si>
+    <t>$3,751.85</t>
+  </si>
+  <si>
+    <t>$3,593.59</t>
+  </si>
+  <si>
+    <t>$3,554.10</t>
+  </si>
+  <si>
+    <t>$3,240.74</t>
+  </si>
+  <si>
+    <t>$3,060.48</t>
+  </si>
+  <si>
+    <t>$2,926.83</t>
+  </si>
+  <si>
+    <t>$2,910.77</t>
+  </si>
+  <si>
+    <t>$2,695.19</t>
+  </si>
+  <si>
+    <t>$2,664.09</t>
+  </si>
+  <si>
+    <t>$2,622.43</t>
+  </si>
+  <si>
+    <t>$2,490.98</t>
+  </si>
+  <si>
+    <t>$2,333.24</t>
+  </si>
+  <si>
+    <t>$2,198.35</t>
+  </si>
+  <si>
+    <t>$1,985.78</t>
+  </si>
+  <si>
+    <t>$1,782.55</t>
+  </si>
+  <si>
+    <t>$1,774.85</t>
+  </si>
+  <si>
+    <t>$1,764.68</t>
+  </si>
+  <si>
+    <t>$1,705.00</t>
+  </si>
+  <si>
+    <t>$1,641.92</t>
+  </si>
+  <si>
+    <t>$1,374.45</t>
+  </si>
+  <si>
+    <t>$1,345.58</t>
+  </si>
+  <si>
+    <t>$1,272.15</t>
+  </si>
+  <si>
+    <t>$1,173.15</t>
+  </si>
+  <si>
+    <t>$1,014.75</t>
+  </si>
+  <si>
+    <t>$808.42</t>
   </si>
 </sst>
 </file>
@@ -676,7 +875,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -688,7 +887,7 @@
         <v>42</v>
       </c>
       <c r="E2">
-        <v>470</v>
+        <v>588</v>
       </c>
       <c r="F2" t="s">
         <v>56</v>
@@ -696,7 +895,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -705,10 +904,10 @@
         <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E3">
-        <v>562</v>
+        <v>470</v>
       </c>
       <c r="F3" t="s">
         <v>57</v>
@@ -716,19 +915,19 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E4">
-        <v>583</v>
+        <v>562</v>
       </c>
       <c r="F4" t="s">
         <v>58</v>
@@ -736,7 +935,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -745,10 +944,10 @@
         <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E5">
-        <v>622</v>
+        <v>583</v>
       </c>
       <c r="F5" t="s">
         <v>59</v>
@@ -756,19 +955,19 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6">
-        <v>456</v>
+        <v>622</v>
       </c>
       <c r="F6" t="s">
         <v>60</v>
@@ -776,7 +975,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
-        <v>132</v>
+        <v>107</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -785,10 +984,10 @@
         <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E7">
-        <v>420</v>
+        <v>456</v>
       </c>
       <c r="F7" t="s">
         <v>61</v>
@@ -796,19 +995,19 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E8">
-        <v>489</v>
+        <v>420</v>
       </c>
       <c r="F8" t="s">
         <v>62</v>
@@ -816,19 +1015,19 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E9">
-        <v>364</v>
+        <v>489</v>
       </c>
       <c r="F9" t="s">
         <v>63</v>
@@ -836,7 +1035,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10">
-        <v>110</v>
+        <v>131</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
@@ -848,7 +1047,7 @@
         <v>42</v>
       </c>
       <c r="E10">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="F10" t="s">
         <v>64</v>
@@ -856,19 +1055,19 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B11" t="s">
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E11">
-        <v>455</v>
+        <v>360</v>
       </c>
       <c r="F11" t="s">
         <v>65</v>
@@ -876,19 +1075,19 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E12">
-        <v>359</v>
+        <v>455</v>
       </c>
       <c r="F12" t="s">
         <v>66</v>
@@ -896,19 +1095,19 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="B13" t="s">
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="E13">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="F13" t="s">
         <v>67</v>
@@ -916,19 +1115,19 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B14" t="s">
         <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D14" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E14">
-        <v>354</v>
+        <v>367</v>
       </c>
       <c r="F14" t="s">
         <v>68</v>
@@ -936,19 +1135,19 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B15" t="s">
         <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D15" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="E15">
-        <v>273</v>
+        <v>354</v>
       </c>
       <c r="F15" t="s">
         <v>69</v>
@@ -956,7 +1155,7 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="B16" t="s">
         <v>20</v>
@@ -965,10 +1164,10 @@
         <v>39</v>
       </c>
       <c r="D16" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E16">
-        <v>324</v>
+        <v>273</v>
       </c>
       <c r="F16" t="s">
         <v>70</v>
@@ -976,7 +1175,7 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="B17" t="s">
         <v>21</v>
@@ -985,10 +1184,10 @@
         <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E17">
-        <v>239</v>
+        <v>324</v>
       </c>
       <c r="F17" t="s">
         <v>71</v>
@@ -996,19 +1195,19 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="B18" t="s">
         <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E18">
-        <v>379</v>
+        <v>239</v>
       </c>
       <c r="F18" t="s">
         <v>72</v>
@@ -1016,19 +1215,19 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="B19" t="s">
         <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D19" t="s">
         <v>51</v>
       </c>
       <c r="E19">
-        <v>355</v>
+        <v>379</v>
       </c>
       <c r="F19" t="s">
         <v>73</v>
@@ -1036,19 +1235,19 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B20" t="s">
         <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E20">
-        <v>571</v>
+        <v>355</v>
       </c>
       <c r="F20" t="s">
         <v>74</v>
@@ -1056,19 +1255,19 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="B21" t="s">
         <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D21" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="E21">
-        <v>249</v>
+        <v>571</v>
       </c>
       <c r="F21" t="s">
         <v>75</v>
@@ -1076,19 +1275,19 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="B22" t="s">
         <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D22" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E22">
-        <v>463</v>
+        <v>249</v>
       </c>
       <c r="F22" t="s">
         <v>76</v>
@@ -1096,19 +1295,19 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="B23" t="s">
         <v>27</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23" t="s">
         <v>52</v>
       </c>
       <c r="E23">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="F23" t="s">
         <v>77</v>
@@ -1116,19 +1315,19 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B24" t="s">
         <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D24" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E24">
-        <v>207</v>
+        <v>461</v>
       </c>
       <c r="F24" t="s">
         <v>78</v>
@@ -1136,7 +1335,7 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="B25" t="s">
         <v>29</v>
@@ -1145,10 +1344,10 @@
         <v>39</v>
       </c>
       <c r="D25" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E25">
-        <v>620</v>
+        <v>207</v>
       </c>
       <c r="F25" t="s">
         <v>79</v>
@@ -1156,19 +1355,19 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B26" t="s">
         <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D26" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E26">
-        <v>214</v>
+        <v>620</v>
       </c>
       <c r="F26" t="s">
         <v>80</v>
@@ -1176,19 +1375,19 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="B27" t="s">
         <v>31</v>
       </c>
       <c r="C27" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D27" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="E27">
-        <v>238</v>
+        <v>214</v>
       </c>
       <c r="F27" t="s">
         <v>81</v>
@@ -1196,19 +1395,19 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="B28" t="s">
         <v>32</v>
       </c>
       <c r="C28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D28" t="s">
         <v>54</v>
       </c>
       <c r="E28">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="F28" t="s">
         <v>82</v>
@@ -1216,19 +1415,19 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="B29" t="s">
         <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E29">
-        <v>257</v>
+        <v>233</v>
       </c>
       <c r="F29" t="s">
         <v>83</v>
@@ -1236,19 +1435,19 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="B30" t="s">
         <v>34</v>
       </c>
       <c r="C30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D30" t="s">
         <v>55</v>
       </c>
       <c r="E30">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="F30" t="s">
         <v>84</v>
@@ -1256,19 +1455,19 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="B31" t="s">
         <v>35</v>
       </c>
       <c r="C31" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D31" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E31">
-        <v>588</v>
+        <v>237</v>
       </c>
       <c r="F31" t="s">
         <v>85</v>
@@ -1282,7 +1481,7 @@
         <v>36</v>
       </c>
       <c r="C32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D32" t="s">
         <v>55</v>
@@ -1340,7 +1539,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2">
         <v>3470</v>
@@ -1351,7 +1550,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>2948</v>
@@ -1380,6 +1579,877 @@
       </c>
       <c r="C5" t="s">
         <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2">
+        <v>109</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2">
+        <v>588</v>
+      </c>
+      <c r="F2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3">
+        <v>125</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3">
+        <v>470</v>
+      </c>
+      <c r="F3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" t="s">
+        <v>95</v>
+      </c>
+      <c r="H3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4">
+        <v>108</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4">
+        <v>562</v>
+      </c>
+      <c r="F4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" t="s">
+        <v>96</v>
+      </c>
+      <c r="H4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5">
+        <v>102</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5">
+        <v>583</v>
+      </c>
+      <c r="F5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" t="s">
+        <v>97</v>
+      </c>
+      <c r="H5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6">
+        <v>101</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6">
+        <v>622</v>
+      </c>
+      <c r="F6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" t="s">
+        <v>98</v>
+      </c>
+      <c r="H6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7">
+        <v>107</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7">
+        <v>456</v>
+      </c>
+      <c r="F7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" t="s">
+        <v>99</v>
+      </c>
+      <c r="H7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8">
+        <v>132</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8">
+        <v>420</v>
+      </c>
+      <c r="F8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" t="s">
+        <v>100</v>
+      </c>
+      <c r="H8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9">
+        <v>120</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9">
+        <v>489</v>
+      </c>
+      <c r="F9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" t="s">
+        <v>101</v>
+      </c>
+      <c r="H9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10">
+        <v>131</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10">
+        <v>364</v>
+      </c>
+      <c r="F10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" t="s">
+        <v>102</v>
+      </c>
+      <c r="H10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11">
+        <v>110</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11">
+        <v>360</v>
+      </c>
+      <c r="F11" t="s">
+        <v>65</v>
+      </c>
+      <c r="G11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12">
+        <v>117</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12">
+        <v>455</v>
+      </c>
+      <c r="F12" t="s">
+        <v>66</v>
+      </c>
+      <c r="G12" t="s">
+        <v>104</v>
+      </c>
+      <c r="H12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13">
+        <v>129</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13">
+        <v>359</v>
+      </c>
+      <c r="F13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G13" t="s">
+        <v>105</v>
+      </c>
+      <c r="H13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14">
+        <v>124</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14">
+        <v>367</v>
+      </c>
+      <c r="F14" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" t="s">
+        <v>106</v>
+      </c>
+      <c r="H14" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15">
+        <v>118</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15">
+        <v>354</v>
+      </c>
+      <c r="F15" t="s">
+        <v>69</v>
+      </c>
+      <c r="G15" t="s">
+        <v>107</v>
+      </c>
+      <c r="H15" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16">
+        <v>127</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16">
+        <v>273</v>
+      </c>
+      <c r="F16" t="s">
+        <v>70</v>
+      </c>
+      <c r="G16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H16" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17">
+        <v>112</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17">
+        <v>324</v>
+      </c>
+      <c r="F17" t="s">
+        <v>71</v>
+      </c>
+      <c r="G17" t="s">
+        <v>109</v>
+      </c>
+      <c r="H17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18">
+        <v>130</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18">
+        <v>239</v>
+      </c>
+      <c r="F18" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" t="s">
+        <v>110</v>
+      </c>
+      <c r="H18" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19">
+        <v>119</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19">
+        <v>379</v>
+      </c>
+      <c r="F19" t="s">
+        <v>73</v>
+      </c>
+      <c r="G19" t="s">
+        <v>111</v>
+      </c>
+      <c r="H19" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20">
+        <v>111</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20">
+        <v>355</v>
+      </c>
+      <c r="F20" t="s">
+        <v>74</v>
+      </c>
+      <c r="G20" t="s">
+        <v>112</v>
+      </c>
+      <c r="H20" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21">
+        <v>106</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21">
+        <v>571</v>
+      </c>
+      <c r="F21" t="s">
+        <v>75</v>
+      </c>
+      <c r="G21" t="s">
+        <v>113</v>
+      </c>
+      <c r="H21" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22">
+        <v>126</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22">
+        <v>249</v>
+      </c>
+      <c r="F22" t="s">
+        <v>76</v>
+      </c>
+      <c r="G22" t="s">
+        <v>114</v>
+      </c>
+      <c r="H22" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23">
+        <v>105</v>
+      </c>
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23">
+        <v>463</v>
+      </c>
+      <c r="F23" t="s">
+        <v>77</v>
+      </c>
+      <c r="G23" t="s">
+        <v>115</v>
+      </c>
+      <c r="H23" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24">
+        <v>122</v>
+      </c>
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24">
+        <v>461</v>
+      </c>
+      <c r="F24" t="s">
+        <v>78</v>
+      </c>
+      <c r="G24" t="s">
+        <v>116</v>
+      </c>
+      <c r="H24" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25">
+        <v>128</v>
+      </c>
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25">
+        <v>207</v>
+      </c>
+      <c r="F25" t="s">
+        <v>79</v>
+      </c>
+      <c r="G25" t="s">
+        <v>117</v>
+      </c>
+      <c r="H25" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26">
+        <v>113</v>
+      </c>
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26">
+        <v>620</v>
+      </c>
+      <c r="F26" t="s">
+        <v>80</v>
+      </c>
+      <c r="G26" t="s">
+        <v>118</v>
+      </c>
+      <c r="H26" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27">
+        <v>116</v>
+      </c>
+      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27">
+        <v>214</v>
+      </c>
+      <c r="F27" t="s">
+        <v>81</v>
+      </c>
+      <c r="G27" t="s">
+        <v>119</v>
+      </c>
+      <c r="H27" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28">
+        <v>104</v>
+      </c>
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28">
+        <v>238</v>
+      </c>
+      <c r="F28" t="s">
+        <v>82</v>
+      </c>
+      <c r="G28" t="s">
+        <v>120</v>
+      </c>
+      <c r="H28" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29">
+        <v>121</v>
+      </c>
+      <c r="B29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" t="s">
+        <v>54</v>
+      </c>
+      <c r="E29">
+        <v>233</v>
+      </c>
+      <c r="F29" t="s">
+        <v>83</v>
+      </c>
+      <c r="G29" t="s">
+        <v>121</v>
+      </c>
+      <c r="H29" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30">
+        <v>103</v>
+      </c>
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" t="s">
+        <v>55</v>
+      </c>
+      <c r="E30">
+        <v>257</v>
+      </c>
+      <c r="F30" t="s">
+        <v>84</v>
+      </c>
+      <c r="G30" t="s">
+        <v>122</v>
+      </c>
+      <c r="H30" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31">
+        <v>123</v>
+      </c>
+      <c r="B31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" t="s">
+        <v>55</v>
+      </c>
+      <c r="E31">
+        <v>237</v>
+      </c>
+      <c r="F31" t="s">
+        <v>85</v>
+      </c>
+      <c r="G31" t="s">
+        <v>123</v>
+      </c>
+      <c r="H31" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32">
+        <v>114</v>
+      </c>
+      <c r="B32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" t="s">
+        <v>55</v>
+      </c>
+      <c r="E32">
+        <v>205</v>
+      </c>
+      <c r="F32" t="s">
+        <v>86</v>
+      </c>
+      <c r="G32" t="s">
+        <v>124</v>
+      </c>
+      <c r="H32" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33">
+        <v>115</v>
+      </c>
+      <c r="B33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" t="s">
+        <v>51</v>
+      </c>
+      <c r="E33">
+        <v>123</v>
+      </c>
+      <c r="F33" t="s">
+        <v>87</v>
+      </c>
+      <c r="G33" t="s">
+        <v>125</v>
+      </c>
+      <c r="H33" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fetch income from excel and make sum on income for grt total income
</commit_message>
<xml_diff>
--- a/excel_data/orders_and_products.xlsx
+++ b/excel_data/orders_and_products.xlsx
@@ -10,13 +10,14 @@
     <sheet name="income" sheetId="1" r:id="rId1"/>
     <sheet name="income_by_category" sheetId="2" r:id="rId2"/>
     <sheet name="charges&amp;passive" sheetId="3" r:id="rId3"/>
+    <sheet name="test" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="160">
   <si>
     <t>Order_item_id</t>
   </si>
@@ -490,6 +491,12 @@
   </si>
   <si>
     <t>$808.42</t>
+  </si>
+  <si>
+    <t>Sheet Name</t>
+  </si>
+  <si>
+    <t>Total Income</t>
   </si>
 </sst>
 </file>
@@ -2455,4 +2462,33 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>159217.9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add a condition for can get all income number , charges and passive ... I am working on it
</commit_message>
<xml_diff>
--- a/excel_data/orders_and_products.xlsx
+++ b/excel_data/orders_and_products.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="income" sheetId="1" r:id="rId1"/>
+    <sheet name="all_income" sheetId="1" r:id="rId1"/>
     <sheet name="income_by_category" sheetId="2" r:id="rId2"/>
     <sheet name="charges&amp;passive" sheetId="3" r:id="rId3"/>
-    <sheet name="test" sheetId="4" r:id="rId4"/>
+    <sheet name="total_income" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -493,7 +493,7 @@
     <t>$808.42</t>
   </si>
   <si>
-    <t>Sheet Name</t>
+    <t>Opirations</t>
   </si>
   <si>
     <t>Total Income</t>
@@ -2485,7 +2485,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>159217.9</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finsh total_income sheet .. and finsh the mini data anaylise project
</commit_message>
<xml_diff>
--- a/excel_data/orders_and_products.xlsx
+++ b/excel_data/orders_and_products.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="160">
   <si>
     <t>Order_item_id</t>
   </si>
@@ -283,19 +283,19 @@
     <t>$1,469.85</t>
   </si>
   <si>
-    <t>$62,286.50</t>
-  </si>
-  <si>
-    <t>$42,746.00</t>
-  </si>
-  <si>
-    <t>$38,137.75</t>
-  </si>
-  <si>
-    <t>$19,138.00</t>
-  </si>
-  <si>
-    <t>chargers</t>
+    <t>$49,462.70</t>
+  </si>
+  <si>
+    <t>$46,720.65</t>
+  </si>
+  <si>
+    <t>$34,796.80</t>
+  </si>
+  <si>
+    <t>$28,237.75</t>
+  </si>
+  <si>
+    <t>charges</t>
   </si>
   <si>
     <t>passive</t>
@@ -496,7 +496,7 @@
     <t>Opirations</t>
   </si>
   <si>
-    <t>Total Income</t>
+    <t>Total cache</t>
   </si>
 </sst>
 </file>
@@ -1546,10 +1546,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2">
-        <v>3470</v>
+        <v>2948</v>
       </c>
       <c r="C2" t="s">
         <v>88</v>
@@ -1557,10 +1557,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3">
-        <v>2948</v>
+        <v>3470</v>
       </c>
       <c r="C3" t="s">
         <v>89</v>
@@ -2466,7 +2466,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2485,7 +2485,23 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>159217.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3">
+        <v>71648.09</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4">
+        <v>87569.89999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>